<commit_message>
code for comparision -needs to be fixxed  else EDE to ED done
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/Input_TestData_laxmi.xlsx
+++ b/CTDC_Automation/TestData/Input_TestData_laxmi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\Katalon_Automation\DataCommons_Automation\CTDC_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\Katalon421\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2B85D9-0308-42A9-BE26-D9B45BBE120C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0562BEC-3DC5-4378-A66D-2A2F3CB7318B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="115">
   <si>
     <t>Environment</t>
   </si>
@@ -230,12 +230,6 @@
     <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WITH DISTINCT c AS c, p, s, demo, diag RETURN c.case_id AS case_id, s.clinical_study_designation AS study_code, s.clinical_study_type AS study_type, demo.breed AS breed, diag.disease_term AS diagnosis, diag.stage_of_disease AS stage_of_disease,demo.patient_age_at_enrollment AS age, demo.sex AS sex, demo.neutered_indicator AS neutered_status</t>
   </si>
   <si>
-    <t>bolt://ncidb-q325-c.nci.nih.gov:7687</t>
-  </si>
-  <si>
-    <t>C:\\Data\\TestOutPutTrials_cases_try.xlsx</t>
-  </si>
-  <si>
     <t xml:space="preserve">ICDC Cases query </t>
   </si>
   <si>
@@ -372,6 +366,18 @@
   </si>
   <si>
     <t>Select_case_checkbox</t>
+  </si>
+  <si>
+    <t>C:\\Data\\Test_outCanine.xlsx</t>
+  </si>
+  <si>
+    <t>http://ncias-q2251-c.nci.nih.gov:7474/</t>
+  </si>
+  <si>
+    <t>bolt://ncias-q2251-c.nci.nih.gov:7687</t>
+  </si>
+  <si>
+    <t>compare</t>
   </si>
 </sst>
 </file>
@@ -424,10 +430,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -744,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +762,7 @@
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="70.28515625" customWidth="1"/>
   </cols>
@@ -794,7 +801,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -803,15 +810,21 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="/" xr:uid="{EC05AA3E-1C89-4924-A0FA-C4301489A4D3}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{39C84C9D-3809-4840-9002-E08B972E2AAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -820,7 +833,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,7 +920,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -922,7 +935,7 @@
         <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -939,34 +952,34 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
         <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="K4" t="s">
         <v>21</v>
@@ -974,34 +987,34 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
         <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="K5" t="s">
         <v>21</v>
@@ -1015,7 +1028,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
         <v>76</v>
@@ -1027,16 +1040,16 @@
         <v>29</v>
       </c>
       <c r="G6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
         <v>84</v>
-      </c>
-      <c r="H6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" t="s">
-        <v>86</v>
       </c>
       <c r="K6" t="s">
         <v>21</v>
@@ -1050,7 +1063,7 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
         <v>80</v>
@@ -1062,7 +1075,7 @@
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H7" t="s">
         <v>29</v>
@@ -1071,7 +1084,7 @@
         <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K7" t="s">
         <v>21</v>
@@ -1085,10 +1098,10 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -1097,7 +1110,7 @@
         <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="H8" t="s">
         <v>29</v>
@@ -1106,24 +1119,21 @@
         <v>29</v>
       </c>
       <c r="J8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K8" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -1132,18 +1142,18 @@
         <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
         <v>29</v>
       </c>
       <c r="I9" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="J9" t="s">
-        <v>86</v>
-      </c>
-      <c r="K9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1151,8 +1161,8 @@
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>96</v>
+      <c r="B10" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -1172,35 +1182,29 @@
       <c r="H10" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>21</v>
+      <c r="I10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" location="/cases" display="https://caninecommons.cancer.gov/ - /cases" xr:uid="{76F46532-3B9B-4B59-B4D7-59C6259F9AE1}"/>
-    <hyperlink ref="B4" r:id="rId2" location="/cases" display="https://caninecommons.cancer.gov/ - /cases" xr:uid="{9B77CAEF-54D8-4A48-96E0-93A20E7147F5}"/>
-    <hyperlink ref="B5" r:id="rId3" location="/cases" display="https://caninecommons.cancer.gov/ - /cases" xr:uid="{250A6AB4-0966-4884-900D-3E4950FA6C16}"/>
-    <hyperlink ref="B10" r:id="rId4" location="/cases" display="https://caninecommons.cancer.gov/ - /cases" xr:uid="{F6EA5BF8-B2E9-489E-B903-00BC952ABCD7}"/>
+    <hyperlink ref="B3" r:id="rId1" location="/cases" display="https://caninecommons.cancer.gov/ - /cases" xr:uid="{D2FAD7B9-EC36-4641-80B9-942E2777CC35}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E60AE08-F6F7-4D66-9A20-44C6071A5BA3}">
-  <dimension ref="A2:K84"/>
+  <dimension ref="A2:K96"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:XFD71"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:XFD89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1340,7 @@
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
@@ -1504,7 +1508,7 @@
         <v>27</v>
       </c>
       <c r="G54" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H54" t="s">
         <v>31</v>
@@ -1533,13 +1537,13 @@
         <v>7</v>
       </c>
       <c r="E55" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F55" t="s">
         <v>27</v>
       </c>
       <c r="G55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H55" t="s">
         <v>31</v>
@@ -1559,19 +1563,19 @@
         <v>37</v>
       </c>
       <c r="C58" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D58" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E58" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F58" t="s">
         <v>27</v>
       </c>
       <c r="G58" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H58" t="s">
         <v>31</v>
@@ -1594,19 +1598,19 @@
         <v>37</v>
       </c>
       <c r="C59" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D59" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E59" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F59" t="s">
         <v>27</v>
       </c>
       <c r="G59" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H59" t="s">
         <v>31</v>
@@ -1629,19 +1633,19 @@
         <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D60" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E60" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F60" t="s">
         <v>27</v>
       </c>
       <c r="G60" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H60" t="s">
         <v>31</v>
@@ -1664,19 +1668,19 @@
         <v>37</v>
       </c>
       <c r="C61" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D61" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E61" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F61" t="s">
         <v>27</v>
       </c>
       <c r="G61" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H61" t="s">
         <v>31</v>
@@ -1781,7 +1785,7 @@
         <v>27</v>
       </c>
       <c r="G64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H64" t="s">
         <v>31</v>
@@ -1816,7 +1820,7 @@
         <v>27</v>
       </c>
       <c r="G65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H65" t="s">
         <v>31</v>
@@ -1836,7 +1840,7 @@
         <v>29</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C66" t="s">
         <v>29</v>
@@ -1860,10 +1864,10 @@
         <v>29</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -1871,31 +1875,31 @@
         <v>3</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C67" t="s">
+        <v>107</v>
+      </c>
+      <c r="D67" t="s">
+        <v>108</v>
+      </c>
+      <c r="E67" t="s">
+        <v>29</v>
+      </c>
+      <c r="F67" t="s">
+        <v>29</v>
+      </c>
+      <c r="G67" t="s">
+        <v>29</v>
+      </c>
+      <c r="H67" t="s">
         <v>109</v>
       </c>
-      <c r="D67" t="s">
+      <c r="I67" t="s">
+        <v>29</v>
+      </c>
+      <c r="J67" t="s">
         <v>110</v>
-      </c>
-      <c r="E67" t="s">
-        <v>29</v>
-      </c>
-      <c r="F67" t="s">
-        <v>29</v>
-      </c>
-      <c r="G67" t="s">
-        <v>29</v>
-      </c>
-      <c r="H67" t="s">
-        <v>111</v>
-      </c>
-      <c r="I67" t="s">
-        <v>29</v>
-      </c>
-      <c r="J67" t="s">
-        <v>112</v>
       </c>
       <c r="K67" t="s">
         <v>21</v>
@@ -1906,22 +1910,22 @@
         <v>3</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C68" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D68" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E68" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F68" t="s">
         <v>27</v>
       </c>
       <c r="G68" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H68" t="s">
         <v>31</v>
@@ -1941,22 +1945,22 @@
         <v>3</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C69" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D69" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F69" t="s">
         <v>27</v>
       </c>
       <c r="G69" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H69" t="s">
         <v>31</v>
@@ -1976,22 +1980,22 @@
         <v>3</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C70" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D70" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E70" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F70" t="s">
         <v>27</v>
       </c>
       <c r="G70" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H70" t="s">
         <v>31</v>
@@ -2011,22 +2015,22 @@
         <v>3</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C71" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D71" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E71" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F71" t="s">
         <v>27</v>
       </c>
       <c r="G71" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H71" t="s">
         <v>31</v>
@@ -2043,63 +2047,63 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D76" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D77" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D78" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D79" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D80" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D81" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D82" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -2107,33 +2111,313 @@
         <v>3</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C84" t="s">
+        <v>107</v>
+      </c>
+      <c r="D84" t="s">
+        <v>108</v>
+      </c>
+      <c r="E84" t="s">
+        <v>29</v>
+      </c>
+      <c r="F84" t="s">
+        <v>29</v>
+      </c>
+      <c r="G84" t="s">
+        <v>29</v>
+      </c>
+      <c r="H84" t="s">
+        <v>109</v>
+      </c>
+      <c r="I84" t="s">
+        <v>29</v>
+      </c>
+      <c r="J84" t="s">
+        <v>110</v>
+      </c>
+      <c r="K84" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C89" t="s">
+        <v>85</v>
+      </c>
+      <c r="D89" t="s">
+        <v>85</v>
+      </c>
+      <c r="E89" t="s">
         <v>96</v>
       </c>
-      <c r="C84" t="s">
-        <v>109</v>
-      </c>
-      <c r="D84" t="s">
-        <v>110</v>
-      </c>
-      <c r="E84" t="s">
-        <v>29</v>
-      </c>
-      <c r="F84" t="s">
-        <v>29</v>
-      </c>
-      <c r="G84" t="s">
-        <v>29</v>
-      </c>
-      <c r="H84" t="s">
-        <v>111</v>
-      </c>
-      <c r="I84" t="s">
-        <v>29</v>
-      </c>
-      <c r="J84" t="s">
-        <v>112</v>
-      </c>
-      <c r="K84" t="s">
+      <c r="F89" t="s">
+        <v>27</v>
+      </c>
+      <c r="G89" t="s">
+        <v>97</v>
+      </c>
+      <c r="H89" t="s">
+        <v>31</v>
+      </c>
+      <c r="I89" t="s">
+        <v>29</v>
+      </c>
+      <c r="J89" t="s">
+        <v>30</v>
+      </c>
+      <c r="K89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C90" t="s">
+        <v>22</v>
+      </c>
+      <c r="D90" t="s">
+        <v>7</v>
+      </c>
+      <c r="E90" t="s">
+        <v>8</v>
+      </c>
+      <c r="F90" t="s">
+        <v>27</v>
+      </c>
+      <c r="G90" t="s">
+        <v>67</v>
+      </c>
+      <c r="H90" t="s">
+        <v>31</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J90" t="s">
+        <v>30</v>
+      </c>
+      <c r="K90" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C91" t="s">
+        <v>85</v>
+      </c>
+      <c r="D91" t="s">
+        <v>85</v>
+      </c>
+      <c r="E91" t="s">
+        <v>96</v>
+      </c>
+      <c r="F91" t="s">
+        <v>27</v>
+      </c>
+      <c r="G91" t="s">
+        <v>97</v>
+      </c>
+      <c r="H91" t="s">
+        <v>31</v>
+      </c>
+      <c r="I91" t="s">
+        <v>29</v>
+      </c>
+      <c r="J91" t="s">
+        <v>30</v>
+      </c>
+      <c r="K91" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C92" t="s">
+        <v>85</v>
+      </c>
+      <c r="D92" t="s">
+        <v>85</v>
+      </c>
+      <c r="E92" t="s">
+        <v>90</v>
+      </c>
+      <c r="F92" t="s">
+        <v>27</v>
+      </c>
+      <c r="G92" t="s">
+        <v>98</v>
+      </c>
+      <c r="H92" t="s">
+        <v>31</v>
+      </c>
+      <c r="I92" t="s">
+        <v>29</v>
+      </c>
+      <c r="J92" t="s">
+        <v>30</v>
+      </c>
+      <c r="K92" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>29</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" t="s">
+        <v>77</v>
+      </c>
+      <c r="D93" t="s">
+        <v>74</v>
+      </c>
+      <c r="E93" t="s">
+        <v>29</v>
+      </c>
+      <c r="F93" t="s">
+        <v>29</v>
+      </c>
+      <c r="G93" t="s">
+        <v>82</v>
+      </c>
+      <c r="H93" t="s">
+        <v>29</v>
+      </c>
+      <c r="I93" t="s">
+        <v>29</v>
+      </c>
+      <c r="J93" t="s">
+        <v>84</v>
+      </c>
+      <c r="K93" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>29</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C94" t="s">
+        <v>75</v>
+      </c>
+      <c r="D94" t="s">
+        <v>78</v>
+      </c>
+      <c r="E94" t="s">
+        <v>29</v>
+      </c>
+      <c r="F94" t="s">
+        <v>29</v>
+      </c>
+      <c r="G94" t="s">
+        <v>83</v>
+      </c>
+      <c r="H94" t="s">
+        <v>29</v>
+      </c>
+      <c r="I94" t="s">
+        <v>29</v>
+      </c>
+      <c r="J94" t="s">
+        <v>84</v>
+      </c>
+      <c r="K94" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>29</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C95" t="s">
+        <v>72</v>
+      </c>
+      <c r="D95" t="s">
+        <v>76</v>
+      </c>
+      <c r="E95" t="s">
+        <v>29</v>
+      </c>
+      <c r="F95" t="s">
+        <v>29</v>
+      </c>
+      <c r="G95" t="s">
+        <v>73</v>
+      </c>
+      <c r="H95" t="s">
+        <v>29</v>
+      </c>
+      <c r="I95" t="s">
+        <v>29</v>
+      </c>
+      <c r="J95" t="s">
+        <v>84</v>
+      </c>
+      <c r="K95" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>29</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C96" t="s">
+        <v>79</v>
+      </c>
+      <c r="D96" t="s">
+        <v>80</v>
+      </c>
+      <c r="E96" t="s">
+        <v>29</v>
+      </c>
+      <c r="F96" t="s">
+        <v>29</v>
+      </c>
+      <c r="G96" t="s">
+        <v>81</v>
+      </c>
+      <c r="H96" t="s">
+        <v>29</v>
+      </c>
+      <c r="I96" t="s">
+        <v>29</v>
+      </c>
+      <c r="J96" t="s">
+        <v>84</v>
+      </c>
+      <c r="K96" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2158,8 +2442,12 @@
     <hyperlink ref="B69" r:id="rId17" location="/cases" display="https://caninecommons.cancer.gov/ - /cases" xr:uid="{A4EF0D70-55F6-4146-941D-0111CF05AE45}"/>
     <hyperlink ref="B71" r:id="rId18" location="/cases" display="https://caninecommons.cancer.gov/ - /cases" xr:uid="{F5F94C96-DC2D-4109-A5DF-ADD8D38037D2}"/>
     <hyperlink ref="B70" r:id="rId19" location="/cases" display="https://caninecommons.cancer.gov/ - /cases" xr:uid="{56EF8542-6EE9-4B77-87AB-6ADFE6CA0335}"/>
+    <hyperlink ref="B90" r:id="rId20" location="/cases" display="https://caninecommons.cancer.gov/ - /cases" xr:uid="{3371F7D8-D55A-4CA9-A5A4-460523FC1F48}"/>
+    <hyperlink ref="B91" r:id="rId21" location="/cases" display="https://caninecommons.cancer.gov/ - /cases" xr:uid="{7658CB26-462B-46E0-ACA5-733524BF211E}"/>
+    <hyperlink ref="B92" r:id="rId22" location="/cases" display="https://caninecommons.cancer.gov/ - /cases" xr:uid="{9C26A072-DE6A-4549-87FD-A2B8446F03E5}"/>
+    <hyperlink ref="B89" r:id="rId23" location="/cases" display="https://caninecommons.cancer.gov/ - /cases" xr:uid="{F3E8BB13-45E4-4FD1-9A2B-271C35E346CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId20"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
preDemo - added comparecode_L- going to work on write webdata to excel and then comparison will be done
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/Input_TestData_laxmi.xlsx
+++ b/CTDC_Automation/TestData/Input_TestData_laxmi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\Katalon421\DataCommons_Automation\CTDC_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Documents\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0562BEC-3DC5-4378-A66D-2A2F3CB7318B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D034EC7-163A-4337-975F-3FA2474C2A49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="115">
   <si>
     <t>Environment</t>
   </si>
@@ -368,16 +368,16 @@
     <t>Select_case_checkbox</t>
   </si>
   <si>
-    <t>C:\\Data\\Test_outCanine.xlsx</t>
-  </si>
-  <si>
-    <t>http://ncias-q2251-c.nci.nih.gov:7474/</t>
+    <t>compare</t>
+  </si>
+  <si>
+    <t>C:\Users\radhakrishnang2\Documents\DataCommons_Automation\CTDC_Automation\TestData\CanineDatafromNeo4j.xlsx</t>
   </si>
   <si>
     <t>bolt://ncias-q2251-c.nci.nih.gov:7687</t>
   </si>
   <si>
-    <t>compare</t>
+    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WITH DISTINCT c AS c, p, s, demo, diag RETURN c.case_id AS `Case ID`, s.clinical_study_designation AS `Study Code`, s.clinical_study_type AS `Study Type`, demo.breed AS Breed, diag.disease_term AS Diagnosis, diag.stage_of_disease AS `Stage of Disease`,demo.patient_age_at_enrollment AS Age, demo.sex AS Sex, demo.neutered_indicator AS `Neutered Status`</t>
   </si>
 </sst>
 </file>
@@ -753,21 +753,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="59.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="70.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="4" max="4" width="59.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="70.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -790,7 +790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -810,18 +810,16 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D4" s="1" t="s">
         <v>112</v>
       </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="/" xr:uid="{EC05AA3E-1C89-4924-A0FA-C4301489A4D3}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{39C84C9D-3809-4840-9002-E08B972E2AAC}"/>
+    <hyperlink ref="D2" r:id="rId2" display="http://ncias-q2251-c.nci.nih.gov:7687" xr:uid="{4381B5EF-3CC8-41D8-98D4-CF7F9613D425}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -832,20 +830,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C468257-9521-42A0-A4DB-E0691FA7FE45}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="76" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
-    <col min="7" max="7" width="99.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.7265625" customWidth="1"/>
+    <col min="7" max="7" width="99.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -880,7 +878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -915,7 +913,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -950,7 +948,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -985,7 +983,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1020,7 +1018,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1055,7 +1053,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1090,7 +1088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1122,7 +1120,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1148,7 +1146,7 @@
         <v>29</v>
       </c>
       <c r="I9" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="J9" t="s">
         <v>62</v>
@@ -1157,7 +1155,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1186,7 +1184,7 @@
         <v>29</v>
       </c>
       <c r="J10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1207,15 +1205,15 @@
       <selection activeCell="A89" sqref="A89:XFD89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1232,7 +1230,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>41</v>
       </c>
@@ -1243,7 +1241,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>45</v>
       </c>
@@ -1251,7 +1249,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>47</v>
       </c>
@@ -1259,12 +1257,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>43</v>
       </c>
@@ -1272,42 +1270,42 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D34" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
         <v>56</v>
       </c>
@@ -1315,12 +1313,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D36" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D38" t="s">
         <v>56</v>
       </c>
@@ -1328,27 +1326,27 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D40" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D42" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.35">
       <c r="D46" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -1383,7 +1381,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -1418,7 +1416,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1453,7 +1451,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1488,7 +1486,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -1523,7 +1521,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -1555,7 +1553,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -1590,7 +1588,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1625,7 +1623,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -1660,7 +1658,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>3</v>
       </c>
@@ -1695,7 +1693,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>29</v>
       </c>
@@ -1730,7 +1728,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>29</v>
       </c>
@@ -1765,7 +1763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -1800,7 +1798,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -1835,7 +1833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>29</v>
       </c>
@@ -1870,7 +1868,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -1905,7 +1903,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>3</v>
       </c>
@@ -1940,7 +1938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -1975,7 +1973,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -2010,7 +2008,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>3</v>
       </c>
@@ -2045,12 +2043,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C73" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C76" t="s">
         <v>96</v>
       </c>
@@ -2058,7 +2056,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C77" t="s">
         <v>90</v>
       </c>
@@ -2066,7 +2064,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C78" t="s">
         <v>99</v>
       </c>
@@ -2074,7 +2072,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C79" t="s">
         <v>101</v>
       </c>
@@ -2082,7 +2080,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C80" t="s">
         <v>93</v>
       </c>
@@ -2090,7 +2088,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C81" t="s">
         <v>103</v>
       </c>
@@ -2098,7 +2096,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C82" t="s">
         <v>105</v>
       </c>
@@ -2106,7 +2104,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>3</v>
       </c>
@@ -2141,7 +2139,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -2176,7 +2174,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>3</v>
       </c>
@@ -2211,7 +2209,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>3</v>
       </c>
@@ -2246,7 +2244,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>3</v>
       </c>
@@ -2281,7 +2279,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>29</v>
       </c>
@@ -2316,7 +2314,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>29</v>
       </c>
@@ -2351,7 +2349,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>29</v>
       </c>
@@ -2386,7 +2384,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
complete workflow for canine including data comparison
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/Input_TestData_laxmi.xlsx
+++ b/CTDC_Automation/TestData/Input_TestData_laxmi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Documents\DataCommons_Automation\CTDC_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D034EC7-163A-4337-975F-3FA2474C2A49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B189A570-6190-4465-A7F3-9D50FFE354EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="117">
   <si>
     <t>Environment</t>
   </si>
@@ -371,13 +371,19 @@
     <t>compare</t>
   </si>
   <si>
-    <t>C:\Users\radhakrishnang2\Documents\DataCommons_Automation\CTDC_Automation\TestData\CanineDatafromNeo4j.xlsx</t>
-  </si>
-  <si>
     <t>bolt://ncias-q2251-c.nci.nih.gov:7687</t>
   </si>
   <si>
     <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WITH DISTINCT c AS c, p, s, demo, diag RETURN c.case_id AS `Case ID`, s.clinical_study_designation AS `Study Code`, s.clinical_study_type AS `Study Type`, demo.breed AS Breed, diag.disease_term AS Diagnosis, diag.stage_of_disease AS `Stage of Disease`,demo.patient_age_at_enrollment AS Age, demo.sex AS Sex, demo.neutered_indicator AS `Neutered Status`</t>
+  </si>
+  <si>
+    <t>WebExcel</t>
+  </si>
+  <si>
+    <t>C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\TestData\CanineDatafromNeo4j.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\TestData\CanineDataWebData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -430,11 +436,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -751,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -765,9 +774,10 @@
     <col min="4" max="4" width="59.26953125" customWidth="1"/>
     <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="70.26953125" customWidth="1"/>
+    <col min="8" max="8" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -789,8 +799,11 @@
       <c r="G1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -801,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -809,11 +822,14 @@
       <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D4" s="1"/>
     </row>
   </sheetData>
@@ -830,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C468257-9521-42A0-A4DB-E0691FA7FE45}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+    <sheetView topLeftCell="G4" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -1146,7 +1162,7 @@
         <v>29</v>
       </c>
       <c r="I9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J9" t="s">
         <v>62</v>

</xml_diff>